<commit_message>
Graph changes and unit type removed
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
+++ b/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC38A290-C332-40CD-B16F-7CB4A33797EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D8096-B11D-4206-9D69-A8F83D8888C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8985" activeTab="4" xr2:uid="{EF3683C4-8501-45B9-86F0-5CD5CE0C2B54}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8985" xr2:uid="{EF3683C4-8501-45B9-86F0-5CD5CE0C2B54}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="1" r:id="rId1"/>
@@ -1090,8 +1090,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="A2:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,6 +1125,9 @@
       <c r="C2" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -1136,6 +1139,9 @@
       <c r="C3" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1147,6 +1153,9 @@
       <c r="C4" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="D4" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1158,7 +1167,9 @@
       <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1170,7 +1181,9 @@
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1182,7 +1195,9 @@
       <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -1194,7 +1209,9 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1266,9 +1283,6 @@
       <c r="C14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1280,9 +1294,6 @@
       <c r="C15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1294,11 +1305,8 @@
       <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>133</v>
       </c>
@@ -1308,11 +1316,8 @@
       <c r="C17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>131</v>
       </c>
@@ -1322,11 +1327,8 @@
       <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>130</v>
       </c>
@@ -1336,11 +1338,8 @@
       <c r="C19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>82</v>
       </c>
@@ -1350,11 +1349,8 @@
       <c r="C20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>78</v>
       </c>
@@ -1365,7 +1361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
@@ -1376,7 +1372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>36</v>
       </c>
@@ -1387,7 +1383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>38</v>
       </c>
@@ -1398,7 +1394,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>40</v>
       </c>
@@ -1409,7 +1405,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
@@ -1420,7 +1416,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
   </sheetData>
@@ -1438,7 +1434,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,7 +1741,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,8 +2332,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Promocode modules has been added
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
+++ b/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\ARCDataTemplete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E795DB2A-FE5E-4B45-B7F9-46E4DDAB2F27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0062812D-A2A3-4C51-9F01-D8D0C843E4F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8985" activeTab="4" xr2:uid="{EF3683C4-8501-45B9-86F0-5CD5CE0C2B54}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{EF3683C4-8501-45B9-86F0-5CD5CE0C2B54}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Waste" sheetId="3" r:id="rId3"/>
     <sheet name="LEEDData" sheetId="7" r:id="rId4"/>
     <sheet name="HumanExp" sheetId="4" r:id="rId5"/>
+    <sheet name="Promocode" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="Dates">'[1]CO2 Readings'!$15:$15</definedName>
@@ -28,12 +29,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="195">
   <si>
     <t>Start</t>
   </si>
@@ -376,12 +378,6 @@
     <t>humanExperience</t>
   </si>
   <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>Jan 31, 2019</t>
   </si>
   <si>
@@ -424,12 +420,6 @@
     <t>0.5</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
@@ -541,38 +531,114 @@
     <t>31</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>27</t>
-  </si>
-  <si>
     <t>15</t>
   </si>
   <si>
     <t>18</t>
+  </si>
+  <si>
+    <t>RatingSystem</t>
+  </si>
+  <si>
+    <t>BuildingOther</t>
+  </si>
+  <si>
+    <t>BuildingNone</t>
+  </si>
+  <si>
+    <t>BuildingLEED</t>
+  </si>
+  <si>
+    <t>CityOther</t>
+  </si>
+  <si>
+    <t>CityNone</t>
+  </si>
+  <si>
+    <t>CityLEED</t>
+  </si>
+  <si>
+    <t>CommunityOther</t>
+  </si>
+  <si>
+    <t>CommunityNone</t>
+  </si>
+  <si>
+    <t>CommunityLEED</t>
+  </si>
+  <si>
+    <t>DiscountedFiftyPrice</t>
+  </si>
+  <si>
+    <t>DiscountedHundredPrice</t>
+  </si>
+  <si>
+    <t>$375.00</t>
+  </si>
+  <si>
+    <t>Schools</t>
+  </si>
+  <si>
+    <t>Transit</t>
+  </si>
+  <si>
+    <t>$5,000.00</t>
+  </si>
+  <si>
+    <t>$1,500.00</t>
+  </si>
+  <si>
+    <t>$ 1,500.00</t>
+  </si>
+  <si>
+    <t>3958880680052718</t>
+  </si>
+  <si>
+    <t>3320160077121355</t>
+  </si>
+  <si>
+    <t>1027012347121352</t>
+  </si>
+  <si>
+    <t>2690189870121353</t>
+  </si>
+  <si>
+    <t>3368813817121348</t>
+  </si>
+  <si>
+    <t>$2,500.00</t>
+  </si>
+  <si>
+    <t>1405106434121348</t>
+  </si>
+  <si>
+    <t>200988524121351</t>
+  </si>
+  <si>
+    <t>$750.00</t>
+  </si>
+  <si>
+    <t>2441644443052552</t>
+  </si>
+  <si>
+    <t>$187.50</t>
+  </si>
+  <si>
+    <t>STGPromocodesFifty</t>
+  </si>
+  <si>
+    <t>STGPromocodeHundred</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,7 +753,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -710,6 +776,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1123,9 +1190,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1144,10 +1211,10 @@
     </row>
     <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>50</v>
@@ -1158,10 +1225,10 @@
     </row>
     <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>49</v>
@@ -1172,10 +1239,10 @@
     </row>
     <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>48</v>
@@ -1186,10 +1253,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -1200,10 +1267,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1214,10 +1281,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -1228,10 +1295,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -1242,10 +1309,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -1254,10 +1321,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -1266,10 +1333,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>10</v>
@@ -1278,10 +1345,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
@@ -1290,10 +1357,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -1302,10 +1369,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
@@ -1313,10 +1380,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>49</v>
@@ -1324,10 +1391,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>48</v>
@@ -1335,10 +1402,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1346,10 +1413,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1357,10 +1424,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>6</v>
@@ -1447,7 +1514,7 @@
       <c r="B27" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:C25">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C25">
     <sortCondition descending="1" ref="A2:A25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,9 +1533,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1484,10 +1551,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>46</v>
@@ -1495,10 +1562,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>47</v>
@@ -1506,10 +1573,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>51</v>
@@ -1517,10 +1584,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -1528,10 +1595,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -1539,10 +1606,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -1550,10 +1617,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>7</v>
@@ -1561,10 +1628,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -1572,10 +1639,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -1583,10 +1650,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>10</v>
@@ -1594,10 +1661,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>11</v>
@@ -1605,10 +1672,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -1616,10 +1683,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>13</v>
@@ -1627,10 +1694,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>47</v>
@@ -1638,10 +1705,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>51</v>
@@ -1649,10 +1716,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>5</v>
@@ -1660,10 +1727,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
@@ -1671,10 +1738,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>6</v>
@@ -1773,10 +1840,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1801,10 +1868,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
@@ -1817,10 +1884,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>24</v>
@@ -1833,10 +1900,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>26</v>
@@ -1849,10 +1916,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>28</v>
@@ -1865,10 +1932,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>29</v>
@@ -1881,10 +1948,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>31</v>
@@ -1897,10 +1964,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>30</v>
@@ -1913,10 +1980,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -1929,10 +1996,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -1943,10 +2010,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>10</v>
@@ -1957,10 +2024,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>32</v>
@@ -1972,10 +2039,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>12</v>
@@ -1986,10 +2053,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>44</v>
@@ -2001,10 +2068,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>24</v>
@@ -2015,10 +2082,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>26</v>
@@ -2029,10 +2096,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>28</v>
@@ -2043,10 +2110,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>29</v>
@@ -2057,10 +2124,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>31</v>
@@ -2168,7 +2235,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D13">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
     <sortCondition ref="B2:B13" customList="January,February,March,April,May,June,July,August,September,October,November,December"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2186,16 +2253,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.2734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.5234375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.37890625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.34765625" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2218,7 +2285,7 @@
         <v>105</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>106</v>
@@ -2244,7 +2311,7 @@
         <v>82</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>97</v>
@@ -2253,19 +2320,19 @@
         <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J2" t="s">
         <v>76</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2276,7 +2343,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>97</v>
@@ -2290,7 +2357,7 @@
         <v>82</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>20</v>
@@ -2304,7 +2371,7 @@
         <v>82</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>96</v>
@@ -2321,7 +2388,7 @@
         <v>34</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2335,12 +2402,12 @@
         <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E8" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>39</v>
@@ -2359,19 +2426,19 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" style="3" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2400,21 +2467,21 @@
         <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="5" t="s">
@@ -2433,16 +2500,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
@@ -2460,16 +2527,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5" t="s">
@@ -2484,16 +2551,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5" t="s">
@@ -2505,16 +2572,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5" t="s">
@@ -2529,16 +2596,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5" t="s">
@@ -2553,16 +2620,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5" t="s">
@@ -2575,16 +2642,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5" t="s">
@@ -2596,16 +2663,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" s="6"/>
       <c r="G10" s="5" t="s">
@@ -2617,16 +2684,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E11" s="6"/>
       <c r="G11" s="5" t="s">
@@ -2636,16 +2703,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12" s="6"/>
       <c r="G12" s="5" t="s">
@@ -2654,16 +2721,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E13" s="6"/>
       <c r="G13" s="5" t="s">
@@ -2672,16 +2739,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="6"/>
       <c r="G14" s="5" t="s">
@@ -2690,16 +2757,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>64</v>
@@ -2707,16 +2774,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>65</v>
@@ -2724,16 +2791,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>66</v>
@@ -2741,16 +2808,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>67</v>
@@ -2758,16 +2825,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>68</v>
@@ -2784,7 +2851,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>69</v>
@@ -2801,7 +2868,7 @@
         <v>58</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>46</v>
@@ -2818,7 +2885,7 @@
         <v>59</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>70</v>
@@ -2835,7 +2902,7 @@
         <v>60</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>71</v>
@@ -2852,7 +2919,7 @@
         <v>61</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>50</v>
@@ -2869,7 +2936,7 @@
         <v>80</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>72</v>
@@ -2886,7 +2953,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>73</v>
@@ -2896,4 +2963,213 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E710388-26F7-426E-B67A-9D4F3F80EEDC}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CITY and Transit AG
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
+++ b/AutomationArc/ARCDataTemplete/ExcelTemplateDataVerificationSheet.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF4440F-29EF-453E-BB17-E85CA1CF8C55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462C6301-B241-4AA2-BDAB-F36A616C44D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="5" xr2:uid="{EF3683C4-8501-45B9-86F0-5CD5CE0C2B54}"/>
   </bookViews>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="203">
   <si>
     <t>Start</t>
   </si>
@@ -646,6 +646,12 @@
   </si>
   <si>
     <t>1000168345</t>
+  </si>
+  <si>
+    <t>STGPromocodeHundredReview</t>
+  </si>
+  <si>
+    <t>STGPromocodesFiftyReview</t>
   </si>
 </sst>
 </file>
@@ -656,7 +662,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1208,9 +1214,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.7109375" style="3" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1551,9 +1557,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1858,10 +1864,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2271,16 +2277,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -2450,13 +2456,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="4" max="4" style="3" width="9.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.140625" style="3" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2985,24 +2991,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E710388-26F7-426E-B67A-9D4F3F80EEDC}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.03125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.96484375" collapsed="true"/>
+    <col min="1" max="1" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>164</v>
       </c>
@@ -3024,8 +3032,14 @@
       <c r="G1" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -3048,7 +3062,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -3071,7 +3085,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>167</v>
       </c>
@@ -3085,7 +3099,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>177</v>
       </c>
@@ -3105,7 +3119,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>178</v>
       </c>
@@ -3125,7 +3139,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>168</v>
       </c>
@@ -3145,7 +3159,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>169</v>
       </c>
@@ -3165,7 +3179,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>170</v>
       </c>
@@ -3179,7 +3193,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3199,7 +3213,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>172</v>
       </c>
@@ -3219,7 +3233,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>173</v>
       </c>

</xml_diff>